<commit_message>
Additional seeds for Displaced Jets test
</commit_message>
<xml_diff>
--- a/development/L1Menu_LLPDisplacedJets_test/PrescaleTable/L1Menu_LLPDisplacedJets_test.xlsx
+++ b/development/L1Menu_LLPDisplacedJets_test/PrescaleTable/L1Menu_LLPDisplacedJets_test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menu_LLPDisplacedJets_test/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{362D5A9F-CF58-C84C-9E4B-8A189BC43DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EC8204-8D8D-FE4B-BA26-0D7CA9BEABC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Index</t>
   </si>
@@ -71,6 +71,18 @@
   </si>
   <si>
     <t>L1_SingleJetDISP60_FWD3p0</t>
+  </si>
+  <si>
+    <t>L1_SingleJetDISP15</t>
+  </si>
+  <si>
+    <t>L1_SingleJetDISP30</t>
+  </si>
+  <si>
+    <t>L1_SingleJetDISP45</t>
+  </si>
+  <si>
+    <t>L1_SingleJetDISP90</t>
   </si>
 </sst>
 </file>
@@ -440,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -696,6 +708,146 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1</v>
+      </c>
+      <c r="I11" s="2">
+        <v>1</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>